<commit_message>
test(cli): add more cli link tests
</commit_message>
<xml_diff>
--- a/tests/cli/link/small_no_link_id_expected_result.xlsx
+++ b/tests/cli/link/small_no_link_id_expected_result.xlsx
@@ -476,7 +476,7 @@
       <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>pidn_date_only</t>
+          <t>small_no_link_id</t>
         </is>
       </c>
       <c r="C1" s="3" t="n"/>
@@ -5966,7 +5966,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="19.2" customWidth="1" min="1" max="1"/>
+    <col width="21.6" customWidth="1" min="1" max="1"/>
     <col width="10.8" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="10.8" customWidth="1" min="4" max="4"/>
@@ -6015,7 +6015,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>pidn_date_only</t>
+          <t>small_no_link_id</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -6035,7 +6035,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>/Users/alee7/ucsf/git/macpie/tests/cli/link/pidn_date_only.xlsx</t>
+          <t>/Users/alee7/ucsf/git/macpie/tests/cli/link/small_no_link_id.xlsx</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -6130,7 +6130,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="19.2" customWidth="1" min="1" max="1"/>
+    <col width="21.6" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="22.8" customWidth="1" min="3" max="3"/>
     <col width="65" customWidth="1" min="4" max="4"/>
@@ -6167,7 +6167,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>pidn_date_only</t>
+          <t>small_no_link_id</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -6194,7 +6194,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>pidn_date_only</t>
+          <t>small_no_link_id</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -6221,7 +6221,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>pidn_date_only</t>
+          <t>small_no_link_id</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">

</xml_diff>